<commit_message>
return ranked pulse order instead of single winning pulse. eliminate unused outputs
</commit_message>
<xml_diff>
--- a/Results/First Pulse/Pulse_Order_vMaster.xlsx
+++ b/Results/First Pulse/Pulse_Order_vMaster.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\danie\dropbox\projects\fellyjish\results\first pulse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Dropbox\Projects\Fellyjish\Results\First Pulse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C030935E-B5A3-4C97-8708-37ACBD0482CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9D090C-B0C0-42F1-8930-0D3FF1C14CB5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="3000" windowWidth="16440" windowHeight="12600" xr2:uid="{A37D13D7-27C4-4692-9953-C5F78D4BD01D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A37D13D7-27C4-4692-9953-C5F78D4BD01D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="First_Pulse" sheetId="1" r:id="rId1"/>
+    <sheet name="RollUp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -373,11 +374,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB08664-F9EE-4342-AD74-80352F281A30}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9076E646-58F0-4B10-9EA2-D28B454A2FE0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>